<commit_message>
Correction of a url link in the form
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-4SF.xlsx
+++ b/form_reporting_templates/Form-4SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78E10E0-86CF-4C8D-98AC-A41B40491EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86BC897-6133-463F-80E3-891201158A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="jbPe6SBLf4oG4Cgxdp2GTHPCnTakxOLusQvs3FLR97ZGw7ZrHwFP80gs+fK1zVtwmXmlsYM45w/LTktaEDAlHA==" workbookSaltValue="+e6btQraNKSRCi9yKssXHA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{742ED9EC-8AD9-42B2-9B99-191B35B67816}"/>
@@ -1221,7 +1221,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,7 +1636,7 @@
       <c r="D38" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jXpyYqRArkJXrgAlkjfNNEuB0uTb3pmspw08KvPpI0kNZzBovU/eEn/yJaTxC03yia1Spn8HgAQo5kXU934a7A==" saltValue="2MD9dtlVejrs/bkmeKifXg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UUXNQ8vsdzNUIs+HaWPaDUqw/Kswl1wqAJsFpUFSxyXfDILbNe+U3TAmzonmZFnL1DEiI+gswJFo6I7srQ2L4g==" saltValue="GAz0fa7kugT9Bx2qPMEH9A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="5">
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
@@ -1644,8 +1644,11 @@
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="C36:G36"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F31 C25 C27:C30 F25:F27 D23 F20 F18 C19:C20" xr:uid="{D97DB983-6157-43A9-ADF0-B303F23C5B2A}">
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F31 C25 C27:C30 C19:C20 D23 F20 F18 F25 F26" xr:uid="{D97DB983-6157-43A9-ADF0-B303F23C5B2A}">
+      <formula1>"&lt;0&gt;0"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27" xr:uid="{75420633-B41C-4713-8CCE-F6E3F5B1EBA7}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1661,7 +1664,7 @@
     <hyperlink ref="C29" r:id="rId9" location="raisings" xr:uid="{70178D33-A777-4FBB-A6A2-D8B94CBA336D}"/>
     <hyperlink ref="C27" r:id="rId10" location="sourcesSF" xr:uid="{71D93F2E-1131-431B-8B9D-FE752AAABCD2}"/>
     <hyperlink ref="C28" r:id="rId11" location="processingsSF" xr:uid="{7137B69B-F308-4CA2-9EFD-570A30893393}"/>
-    <hyperlink ref="F27" r:id="rId12" location="fates" display="Fate of catch sampled" xr:uid="{7A228202-3AA5-42C7-8D30-08152078D86D}"/>
+    <hyperlink ref="F27" r:id="rId12" location="allMeasurementTools" xr:uid="{7A228202-3AA5-42C7-8D30-08152078D86D}"/>
     <hyperlink ref="F26" r:id="rId13" location="allMeasurementTypes" xr:uid="{12743A08-7D0D-4FD3-801E-17FDAB969A4D}"/>
     <hyperlink ref="F31" r:id="rId14" location="fates" xr:uid="{7F16F4B7-0EBD-4CB5-A51B-3B30C421ED01}"/>
   </hyperlinks>

</xml_diff>